<commit_message>
Fixed errors in Excel sheets and R script to match, added Excel formula sheets, corrected UI data to January 2023 revision
</commit_message>
<xml_diff>
--- a/Pivot tables.xlsx
+++ b/Pivot tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrinaxie/Documents/CT DEEP/CLMEDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D95CEBE-CA39-164D-96EC-C877EDB48309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C847E08-A54F-9A45-9B6E-590CAE1C2669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="4" xr2:uid="{8AFA9B2A-EFF2-D34C-BC65-39C095DF88D0}"/>
+    <workbookView xWindow="19160" yWindow="4820" windowWidth="28040" windowHeight="15760" xr2:uid="{8AFA9B2A-EFF2-D34C-BC65-39C095DF88D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Large small category" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Mod distress HES HES-IE" sheetId="6" r:id="rId4"/>
     <sheet name="Raw data" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="36" r:id="rId6"/>
-    <pivotCache cacheId="42" r:id="rId7"/>
-    <pivotCache cacheId="48" r:id="rId8"/>
-    <pivotCache cacheId="54" r:id="rId9"/>
+    <pivotCache cacheId="42" r:id="rId6"/>
+    <pivotCache cacheId="43" r:id="rId7"/>
+    <pivotCache cacheId="44" r:id="rId8"/>
+    <pivotCache cacheId="45" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="24">
   <si>
     <t>UI</t>
   </si>
@@ -170,11 +170,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -193,7 +193,139 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45338.490039351855" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="32" xr:uid="{6E17B337-5870-394A-9F4A-99F0412ECF65}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45372.496352430557" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{1950DAA9-594A-8040-8F15-3D94A323DD33}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A85:F101" sheet="Raw data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Cat" numFmtId="0">
+      <sharedItems count="2">
+        <s v="HES"/>
+        <s v="HES_IE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Collections" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6.6" maxValue="18.100000000000001"/>
+    </cacheField>
+    <cacheField name="Disbursements" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.7" maxValue="33.9"/>
+    </cacheField>
+    <cacheField name="Utility" numFmtId="0">
+      <sharedItems count="2">
+        <s v="UI"/>
+        <s v="ES"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
+        <n v="2019"/>
+        <n v="2020"/>
+        <n v="2021"/>
+        <n v="2022"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Parity" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45372.496352546295" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{F689218A-8ACD-4941-9544-EF4FF2A33BB8}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A67:F83" sheet="Raw data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Cat" numFmtId="0">
+      <sharedItems count="2">
+        <s v="HES"/>
+        <s v="HES_IE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Collections" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.59" maxValue="18.46"/>
+    </cacheField>
+    <cacheField name="Disbursements" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="35.18"/>
+    </cacheField>
+    <cacheField name="Utility" numFmtId="0">
+      <sharedItems count="2">
+        <s v="UI"/>
+        <s v="ES"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
+        <n v="2019"/>
+        <n v="2020"/>
+        <n v="2021"/>
+        <n v="2022"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Parity" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45372.496352662034" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{5DAA79A5-C9BB-C942-B5A2-FCE44EFC50A8}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A49:F65" sheet="Raw data"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Size" numFmtId="0">
+      <sharedItems count="2">
+        <s v="SMALL"/>
+        <s v="LARGE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Collections" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="31.48"/>
+    </cacheField>
+    <cacheField name="Disbursements" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="29.53"/>
+    </cacheField>
+    <cacheField name="Utility" numFmtId="0">
+      <sharedItems count="2">
+        <s v="UI"/>
+        <s v="ES"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
+        <n v="2019"/>
+        <n v="2020"/>
+        <n v="2021"/>
+        <n v="2022"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Parity" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45372.49635277778" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="32" xr:uid="{6E17B337-5870-394A-9F4A-99F0412ECF65}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A14:G46" sheet="Raw data"/>
   </cacheSource>
@@ -242,427 +374,135 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45338.498781828705" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{5DAA79A5-C9BB-C942-B5A2-FCE44EFC50A8}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A49:F65" sheet="Raw data"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="Size" numFmtId="0">
-      <sharedItems count="2">
-        <s v="SMALL"/>
-        <s v="LARGE"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Collections" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="31.48"/>
-    </cacheField>
-    <cacheField name="Disbursements" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="29.53"/>
-    </cacheField>
-    <cacheField name="Utility" numFmtId="0">
-      <sharedItems count="2">
-        <s v="UI"/>
-        <s v="ES"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
-        <n v="2019"/>
-        <n v="2020"/>
-        <n v="2021"/>
-        <n v="2022"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Parity" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45338.505543981482" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{F689218A-8ACD-4941-9544-EF4FF2A33BB8}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A67:F83" sheet="Raw data"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="Cat" numFmtId="0">
-      <sharedItems count="2">
-        <s v="HES"/>
-        <s v="HES_IE"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Collections" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.59" maxValue="18.46"/>
-    </cacheField>
-    <cacheField name="Disbursements" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="35.18"/>
-    </cacheField>
-    <cacheField name="Utility" numFmtId="0">
-      <sharedItems count="2">
-        <s v="UI"/>
-        <s v="ES"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
-        <n v="2019"/>
-        <n v="2020"/>
-        <n v="2021"/>
-        <n v="2022"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Parity" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Xie, Sabrina" refreshedDate="45338.507760532404" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{1950DAA9-594A-8040-8F15-3D94A323DD33}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A85:F101" sheet="Raw data"/>
-  </cacheSource>
-  <cacheFields count="6">
-    <cacheField name="Cat" numFmtId="0">
-      <sharedItems count="2">
-        <s v="HES"/>
-        <s v="HES_IE"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Collections" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6.6" maxValue="18.100000000000001"/>
-    </cacheField>
-    <cacheField name="Disbursements" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.7" maxValue="33.9"/>
-    </cacheField>
-    <cacheField name="Utility" numFmtId="0">
-      <sharedItems count="2">
-        <s v="UI"/>
-        <s v="ES"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2022" count="4">
-        <n v="2019"/>
-        <n v="2020"/>
-        <n v="2021"/>
-        <n v="2022"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Parity" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="32">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="17.66"/>
-    <n v="10.33"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="26.9"/>
-    <n v="30.03"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
+  <r>
+    <x v="0"/>
+    <n v="17.3"/>
+    <n v="5.6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="17.3"/>
+    <n v="27.1"/>
     <x v="0"/>
     <x v="0"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="65.31"/>
-    <n v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="31.02"/>
-    <n v="29.53"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0.73"/>
-    <n v="0.14000000000000001"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <s v="NaN"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="17.559999999999999"/>
-    <n v="8.2200000000000006"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="26.4"/>
-    <n v="22.86"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="65.540000000000006"/>
-    <n v="37.43"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="30.39"/>
-    <n v="18.57"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0.59"/>
-    <n v="0.6"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <n v="7"/>
+    <n v="4.3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
+    <n v="11.9"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="YES"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <s v="NaN"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="17.97"/>
-    <n v="13.9"/>
+    <n v="16.5"/>
+    <n v="4.5"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="16.5"/>
+    <n v="22.1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6.8"/>
+    <n v="2.1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6.8"/>
+    <n v="9.1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="18.100000000000001"/>
+    <n v="6.3"/>
     <x v="0"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="27"/>
-    <n v="26.5"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="59.78"/>
-    <n v="60.74"/>
+    <x v="1"/>
+    <n v="18.100000000000001"/>
+    <n v="33.9"/>
     <x v="0"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="30.41"/>
-    <n v="27.4"/>
-    <x v="0"/>
+    <x v="0"/>
+    <n v="9"/>
+    <n v="3.1"/>
+    <x v="1"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="3.39"/>
-    <n v="2.39"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="1.64"/>
-    <n v="1.76"/>
+    <x v="1"/>
+    <n v="9"/>
+    <n v="9.8000000000000007"/>
     <x v="1"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="16.34"/>
-    <s v="NaN"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="1.1299999999999999"/>
-    <n v="4.12"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="YES"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="17.809999999999999"/>
-    <n v="6.9"/>
+    <x v="0"/>
+    <n v="17.600000000000001"/>
+    <n v="3.8"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="25.59"/>
-    <n v="13.96"/>
+    <x v="1"/>
+    <n v="17.600000000000001"/>
+    <n v="16.899999999999999"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NaN"/>
-    <n v="74.87"/>
-    <x v="0"/>
+    <x v="0"/>
+    <n v="6.6"/>
+    <n v="1.7"/>
+    <x v="1"/>
     <x v="3"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="30.27"/>
-    <n v="22.65"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="4.46"/>
-    <n v="4.72"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6.6"/>
+    <n v="9.1999999999999993"/>
     <x v="1"/>
     <x v="3"/>
     <s v="YES"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="8.57"/>
-    <n v="10.23"/>
-    <x v="1"/>
-    <x v="3"/>
-    <s v="YES"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="18.7"/>
-    <s v="NaN"/>
-    <x v="1"/>
-    <x v="3"/>
-    <s v="NA"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="11.89"/>
-    <n v="11.09"/>
-    <x v="1"/>
-    <x v="3"/>
-    <s v="NO"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -671,131 +511,131 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
   <r>
     <x v="0"/>
-    <n v="20.51"/>
-    <n v="15.67"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="31.48"/>
-    <n v="29.53"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="0.54"/>
-    <n v="0.12"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
+    <n v="17.66"/>
+    <n v="5.39"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="17.66"/>
+    <n v="28.82"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.73"/>
+    <n v="0.05"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0.73"/>
     <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="17.96"/>
+    <n v="3.19"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="17.96"/>
+    <n v="34.01"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.59"/>
     <n v="0"/>
     <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="19.989999999999998"/>
-    <n v="13.05"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="30.87"/>
-    <n v="18.66"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="0.45"/>
-    <n v="0.52"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="YES"/>
-  </r>
-  <r>
-    <x v="1"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="0.59"/>
     <n v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="20.55"/>
-    <n v="20.079999999999998"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="18.46"/>
+    <n v="5.0599999999999996"/>
     <x v="0"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="30.8"/>
-    <n v="29.36"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="2.96"/>
-    <n v="2.29"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="1.1599999999999999"/>
-    <n v="4.12"/>
-    <x v="1"/>
+    <n v="18.46"/>
+    <n v="35.18"/>
+    <x v="0"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="20.010000000000002"/>
-    <n v="9.67"/>
+    <n v="3.41"/>
+    <n v="1.36"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3.41"/>
+    <n v="4.5"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="17.809999999999999"/>
+    <n v="2.5499999999999998"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="30.27"/>
-    <n v="27.31"/>
+    <n v="17.809999999999999"/>
+    <n v="15.82"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="5.45"/>
-    <n v="5.63"/>
+    <n v="4.47"/>
+    <n v="2.81"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4.47"/>
+    <n v="10.23"/>
     <x v="1"/>
     <x v="3"/>
     <s v="YES"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="11.9"/>
-    <n v="11.09"/>
-    <x v="1"/>
-    <x v="3"/>
-    <s v="NO"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -804,63 +644,63 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
   <r>
     <x v="0"/>
-    <n v="17.66"/>
-    <n v="3.26"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="17.66"/>
-    <n v="23.89"/>
+    <n v="20.51"/>
+    <n v="24.16"/>
     <x v="0"/>
     <x v="0"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="0.73"/>
-    <n v="0.05"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="0.73"/>
+    <x v="1"/>
+    <n v="31.48"/>
+    <n v="29.53"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.54"/>
+    <n v="0.12"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
     <n v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="17.96"/>
-    <n v="3.19"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="17.96"/>
-    <n v="34.01"/>
-    <x v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="19.989999999999998"/>
+    <n v="13.05"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="30.87"/>
+    <n v="18.66"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="0.45"/>
+    <n v="0.52"/>
+    <x v="1"/>
     <x v="1"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="0.59"/>
+    <x v="1"/>
     <n v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="0.59"/>
     <n v="0"/>
     <x v="1"/>
     <x v="1"/>
@@ -868,208 +708,375 @@
   </r>
   <r>
     <x v="0"/>
-    <n v="18.46"/>
-    <n v="5.0599999999999996"/>
+    <n v="20.55"/>
+    <n v="20.079999999999998"/>
     <x v="0"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="18.46"/>
-    <n v="35.18"/>
-    <x v="0"/>
+    <n v="30.8"/>
+    <n v="29.36"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2.96"/>
+    <n v="2.29"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1.1599999999999999"/>
+    <n v="4.12"/>
+    <x v="1"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="3.41"/>
-    <n v="1.36"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="3.41"/>
-    <n v="4.5"/>
-    <x v="1"/>
-    <x v="2"/>
-    <s v="YES"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="17.809999999999999"/>
-    <n v="2.5499999999999998"/>
+    <n v="20.010000000000002"/>
+    <n v="9.67"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="17.809999999999999"/>
-    <n v="15.82"/>
+    <n v="30.27"/>
+    <n v="27.31"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="4.47"/>
-    <n v="2.81"/>
-    <x v="1"/>
-    <x v="3"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="4.47"/>
-    <n v="10.23"/>
+    <n v="5.45"/>
+    <n v="5.63"/>
     <x v="1"/>
     <x v="3"/>
     <s v="YES"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="11.9"/>
+    <n v="11.09"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="NO"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
-  <r>
-    <x v="0"/>
-    <n v="17.3"/>
-    <n v="3.2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="17.3"/>
-    <n v="21.4"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="32">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.66"/>
+    <n v="19"/>
     <x v="0"/>
     <x v="0"/>
     <s v="YES"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="7"/>
-    <n v="4.3"/>
-    <x v="1"/>
-    <x v="0"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="7"/>
-    <n v="11.9"/>
-    <x v="1"/>
+    <x v="1"/>
+    <n v="26.9"/>
+    <n v="38.049999999999997"/>
+    <x v="0"/>
     <x v="0"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="16.5"/>
-    <n v="4.5"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="16.5"/>
-    <n v="22.1"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="65.31"/>
+    <n v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="31.02"/>
+    <n v="29.53"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.73"/>
+    <n v="0.14000000000000001"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <s v="NaN"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.559999999999999"/>
+    <n v="8.2200000000000006"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="26.4"/>
+    <n v="22.86"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="65.540000000000006"/>
+    <n v="37.43"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="30.39"/>
+    <n v="18.57"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0.59"/>
+    <n v="0.6"/>
+    <x v="1"/>
     <x v="1"/>
     <s v="YES"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="6.8"/>
-    <n v="2.1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6.8"/>
-    <n v="9.1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="YES"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="18.100000000000001"/>
-    <n v="6.3"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <s v="NaN"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.97"/>
+    <n v="13.9"/>
     <x v="0"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="1"/>
-    <n v="18.100000000000001"/>
-    <n v="33.9"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="27"/>
+    <n v="26.5"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="59.78"/>
+    <n v="60.74"/>
     <x v="0"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="9"/>
-    <n v="3.1"/>
-    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="30.41"/>
+    <n v="27.4"/>
+    <x v="0"/>
     <x v="2"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="1"/>
-    <n v="9"/>
-    <n v="9.8000000000000007"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.39"/>
+    <n v="2.39"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.64"/>
+    <n v="1.76"/>
     <x v="1"/>
     <x v="2"/>
     <s v="YES"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="17.600000000000001"/>
-    <n v="3.8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="16.34"/>
+    <s v="NaN"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.1299999999999999"/>
+    <n v="4.12"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.809999999999999"/>
+    <n v="6.9"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="1"/>
-    <n v="17.600000000000001"/>
-    <n v="16.899999999999999"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="25.59"/>
+    <n v="13.96"/>
     <x v="0"/>
     <x v="3"/>
     <s v="NO"/>
   </r>
   <r>
-    <x v="0"/>
-    <n v="6.6"/>
-    <n v="1.7"/>
-    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="NaN"/>
+    <n v="74.87"/>
+    <x v="0"/>
     <x v="3"/>
-    <s v="NO"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="6.6"/>
-    <n v="9.1999999999999993"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="30.27"/>
+    <n v="22.65"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NO"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.46"/>
+    <n v="4.72"/>
     <x v="1"/>
     <x v="3"/>
     <s v="YES"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="8.57"/>
+    <n v="10.23"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="YES"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="18.7"/>
+    <s v="NaN"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="NA"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="11.89"/>
+    <n v="11.09"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="NO"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{700DBC87-8F79-AF46-A8FF-405DF1F9076D}" name="PivotTable4" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{700DBC87-8F79-AF46-A8FF-405DF1F9076D}" name="PivotTable4" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="7">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
         <item h="1" x="1"/>
@@ -1077,19 +1084,12 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item h="1" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
-        <item x="1"/>
-        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1157,7 +1157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2AF955F3-D086-034A-8F54-62A592773531}" name="PivotTable5" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2AF955F3-D086-034A-8F54-62A592773531}" name="PivotTable5" cacheId="44" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1239,13 +1239,13 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38500CB6-5151-8845-BFFA-FD5F3BE4FC0E}" name="PivotTable6" cacheId="48" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{38500CB6-5151-8845-BFFA-FD5F3BE4FC0E}" name="PivotTable6" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1253,8 +1253,8 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="3">
-        <item h="1" x="1"/>
-        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1321,7 +1321,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B6EE894-477D-844A-AD78-96C6F4CA1B46}" name="PivotTable7" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B6EE894-477D-844A-AD78-96C6F4CA1B46}" name="PivotTable7" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51798FA-66FD-0347-86F7-055FBAC60667}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,31 +1733,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
@@ -1768,58 +1768,58 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2019</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="5">
+        <v>65.31</v>
+      </c>
+      <c r="C6" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>2020</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
+      <c r="B7" s="5">
+        <v>65.540000000000006</v>
+      </c>
+      <c r="C7" s="5">
+        <v>37.43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>2021</v>
       </c>
-      <c r="B8" s="3">
-        <v>1.64</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.76</v>
+      <c r="B8" s="5">
+        <v>59.78</v>
+      </c>
+      <c r="C8" s="5">
+        <v>60.74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>2022</v>
       </c>
-      <c r="B9" s="3">
-        <v>8.57</v>
-      </c>
-      <c r="C9" s="3">
-        <v>10.23</v>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>74.87</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3">
-        <v>10.210000000000001</v>
-      </c>
-      <c r="C10" s="3">
-        <v>11.99</v>
+      <c r="B10" s="5">
+        <v>190.63000000000002</v>
+      </c>
+      <c r="C10" s="5">
+        <v>173.04000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1832,7 +1832,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1843,7 +1843,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
@@ -1851,7 +1851,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -1870,57 +1870,57 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2019</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>31.48</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>29.53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2020</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>30.87</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>18.66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>2021</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>30.8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>29.36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>2022</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>30.27</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>27.31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>123.42</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>104.86</v>
       </c>
     </row>
@@ -1934,7 +1934,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1945,23 +1945,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -1972,58 +1972,58 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2019</v>
       </c>
-      <c r="B5" s="3">
-        <v>17.66</v>
-      </c>
-      <c r="C5" s="3">
-        <v>23.89</v>
+      <c r="B5" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2020</v>
       </c>
-      <c r="B6" s="3">
-        <v>17.96</v>
-      </c>
-      <c r="C6" s="3">
-        <v>34.01</v>
+      <c r="B6" s="5">
+        <v>0.59</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>2021</v>
       </c>
-      <c r="B7" s="3">
-        <v>18.46</v>
-      </c>
-      <c r="C7" s="3">
-        <v>35.18</v>
+      <c r="B7" s="5">
+        <v>3.41</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>2022</v>
       </c>
-      <c r="B8" s="3">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="C8" s="3">
-        <v>15.82</v>
+      <c r="B8" s="5">
+        <v>4.47</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3">
-        <v>71.89</v>
-      </c>
-      <c r="C9" s="3">
-        <v>108.9</v>
+      <c r="B9" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C9" s="5">
+        <v>4.2200000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -2047,7 +2047,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
@@ -2055,7 +2055,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -2063,7 +2063,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
@@ -2074,58 +2074,58 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2019</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>17.3</v>
       </c>
-      <c r="C5" s="3">
-        <v>21.4</v>
+      <c r="C5">
+        <v>27.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2020</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>16.5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>22.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>2021</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>18.100000000000001</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>33.9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>2022</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>17.600000000000001</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>16.899999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>69.5</v>
       </c>
-      <c r="C9" s="3">
-        <v>94.300000000000011</v>
+      <c r="C9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2137,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A517F7-639C-B748-B824-AB51B82DFFCD}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2172,7 +2172,7 @@
         <v>24.87</v>
       </c>
       <c r="B3" s="1">
-        <v>19.920000000000002</v>
+        <v>25.8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -2180,111 +2180,134 @@
       <c r="D3" s="1">
         <v>2019</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>24.1</v>
+        <v>0.34</v>
       </c>
       <c r="B4" s="1">
-        <v>15.32</v>
+        <v>0.06</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>2019</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>24.49</v>
+        <v>24.1</v>
       </c>
       <c r="B5" s="1">
-        <v>22.88</v>
+        <v>15.32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>2021</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>2020</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>28.46</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="B6" s="1">
-        <v>17.329999999999998</v>
+        <v>0.33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>2022</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>2020</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>24.49</v>
+      </c>
+      <c r="B7" s="1">
+        <v>22.88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.34</v>
+        <v>2.29</v>
       </c>
       <c r="B8" s="1">
-        <v>0.06</v>
+        <v>2.93</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>2021</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>0.28999999999999998</v>
+        <v>28.46</v>
       </c>
       <c r="B9" s="1">
-        <v>0.33</v>
+        <v>17.329999999999998</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>2022</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2.29</v>
+        <v>7.83</v>
       </c>
       <c r="B10" s="1">
-        <v>2.93</v>
+        <v>7.41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>2021</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>2022</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>7.83</v>
-      </c>
-      <c r="B11" s="1">
-        <v>7.41</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2022</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2321,7 +2344,7 @@
         <v>17.66</v>
       </c>
       <c r="D15" s="1">
-        <v>10.33</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>0</v>
@@ -2330,7 +2353,7 @@
         <v>2019</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -2344,7 +2367,7 @@
         <v>26.9</v>
       </c>
       <c r="D16" s="1">
-        <v>30.03</v>
+        <v>38.049999999999997</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>0</v>
@@ -3074,7 +3097,7 @@
         <v>20.51</v>
       </c>
       <c r="C50" s="1">
-        <v>15.67</v>
+        <v>24.16</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>0</v>
@@ -3083,7 +3106,7 @@
         <v>2019</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -3414,7 +3437,7 @@
         <v>17.66</v>
       </c>
       <c r="C68" s="1">
-        <v>3.26</v>
+        <v>5.39</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>0</v>
@@ -3434,7 +3457,7 @@
         <v>17.66</v>
       </c>
       <c r="C69" s="1">
-        <v>23.89</v>
+        <v>28.82</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>0</v>
@@ -3754,7 +3777,7 @@
         <v>17.3</v>
       </c>
       <c r="C86" s="1">
-        <v>3.2</v>
+        <v>5.6</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>0</v>
@@ -3774,7 +3797,7 @@
         <v>17.3</v>
       </c>
       <c r="C87" s="1">
-        <v>21.4</v>
+        <v>27.1</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>0</v>

</xml_diff>